<commit_message>
Add plots methods and prints
</commit_message>
<xml_diff>
--- a/output/likelihood_formulas_M1.xlsx
+++ b/output/likelihood_formulas_M1.xlsx
@@ -501,31 +501,31 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1.89</v>
+        <v>1.027</v>
       </c>
       <c r="E2">
-        <v>2.5</v>
+        <v>5.3</v>
       </c>
       <c r="F2">
-        <v>1.510083333333333</v>
+        <v>1.23625</v>
       </c>
       <c r="G2">
-        <v>0.253463701388889</v>
+        <v>0.09761414583333339</v>
       </c>
       <c r="H2">
-        <v>3.573957780154706</v>
+        <v>3.852075156483195</v>
       </c>
       <c r="I2">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J2">
-        <v>0.5960684946711681</v>
+        <v>1.020353483153802</v>
       </c>
       <c r="K2">
-        <v>0.2222337825683584</v>
+        <v>0.1573903470329096</v>
       </c>
       <c r="L2">
-        <v>0.06623327812030051</v>
+        <v>0.08029689440490745</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -539,31 +539,31 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>2.302</v>
+        <v>1.239</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>1.510083333333333</v>
+        <v>1.23625</v>
       </c>
       <c r="G3">
-        <v>0.253463701388889</v>
+        <v>0.09761414583333339</v>
       </c>
       <c r="H3">
-        <v>3.701450363279513</v>
+        <v>3.678867773382904</v>
       </c>
       <c r="I3">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J3">
-        <v>0.2299725999110499</v>
+        <v>1.27684112895035</v>
       </c>
       <c r="K3">
-        <v>0.185441158183911</v>
+        <v>0.3324226319460587</v>
       </c>
       <c r="L3">
-        <v>0.02132319263903514</v>
+        <v>0.2122254443313261</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -577,31 +577,31 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1.1865</v>
+        <v>1.166</v>
       </c>
       <c r="E4">
-        <v>4.25</v>
+        <v>2.5</v>
       </c>
       <c r="F4">
-        <v>1.510083333333333</v>
+        <v>1.23625</v>
       </c>
       <c r="G4">
-        <v>0.253463701388889</v>
+        <v>0.09761414583333339</v>
       </c>
       <c r="H4">
-        <v>3.356261099988927</v>
+        <v>3.738509938318381</v>
       </c>
       <c r="I4">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J4">
-        <v>0.6445377836088926</v>
+        <v>1.245017365128281</v>
       </c>
       <c r="K4">
-        <v>0.2506813729966182</v>
+        <v>0.1943661439160063</v>
       </c>
       <c r="L4">
-        <v>0.08078680827163719</v>
+        <v>0.1209946121842252</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -615,31 +615,31 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1.742</v>
+        <v>0.9089999999999999</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>1.510083333333333</v>
+        <v>1.23625</v>
       </c>
       <c r="G5">
-        <v>0.253463701388889</v>
+        <v>0.09761414583333339</v>
       </c>
       <c r="H5">
-        <v>3.52815947359531</v>
+        <v>3.948483039529583</v>
       </c>
       <c r="I5">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J5">
-        <v>0.7126449980383891</v>
+        <v>0.7377704624374438</v>
       </c>
       <c r="K5">
-        <v>0.3048681233932696</v>
+        <v>0.2465721666239024</v>
       </c>
       <c r="L5">
-        <v>0.108631371598782</v>
+        <v>0.09095683069715947</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -653,31 +653,31 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1.031</v>
+        <v>1.1865</v>
       </c>
       <c r="E6">
-        <v>5.3</v>
+        <v>2.5</v>
       </c>
       <c r="F6">
-        <v>1.510083333333333</v>
+        <v>1.23625</v>
       </c>
       <c r="G6">
-        <v>0.253463701388889</v>
+        <v>0.09761414583333339</v>
       </c>
       <c r="H6">
-        <v>3.308141933299831</v>
+        <v>3.721761111178966</v>
       </c>
       <c r="I6">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J6">
-        <v>0.5038685471710387</v>
+        <v>1.260804627539021</v>
       </c>
       <c r="K6">
-        <v>0.08544366444501053</v>
+        <v>0.1973935966133143</v>
       </c>
       <c r="L6">
-        <v>0.0215261875344386</v>
+        <v>0.1244373800283187</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -691,31 +691,31 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.9089999999999999</v>
+        <v>1.89</v>
       </c>
       <c r="E7">
-        <v>5.5</v>
+        <v>1.8</v>
       </c>
       <c r="F7">
-        <v>1.510083333333333</v>
+        <v>1.23625</v>
       </c>
       <c r="G7">
-        <v>0.253463701388889</v>
+        <v>0.09761414583333339</v>
       </c>
       <c r="H7">
-        <v>3.270389275190059</v>
+        <v>3.146990384711729</v>
       </c>
       <c r="I7">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J7">
-        <v>0.3885245771586974</v>
+        <v>0.143023266457987</v>
       </c>
       <c r="K7">
-        <v>0.06076058050782936</v>
+        <v>0.1749572221769412</v>
       </c>
       <c r="L7">
-        <v>0.0118034894248607</v>
+        <v>0.01251147670308094</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -729,31 +729,31 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>2.446</v>
+        <v>2.171</v>
       </c>
       <c r="E8">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>1.511555555555556</v>
+        <v>1.694111111111111</v>
       </c>
       <c r="G8">
-        <v>0.2361455246913581</v>
+        <v>0.2561913765432099</v>
       </c>
       <c r="H8">
-        <v>3.746010877769736</v>
+        <v>2.917408900508042</v>
       </c>
       <c r="I8">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J8">
-        <v>0.1292358564208007</v>
+        <v>0.5056669539171873</v>
       </c>
       <c r="K8">
-        <v>0.2091736292084351</v>
+        <v>0.06791642735171953</v>
       </c>
       <c r="L8">
-        <v>0.01351636655569956</v>
+        <v>0.01717154646994098</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -767,31 +767,31 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1.07</v>
+        <v>1.8415</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="F9">
-        <v>1.511555555555556</v>
+        <v>1.694111111111111</v>
       </c>
       <c r="G9">
-        <v>0.2361455246913581</v>
+        <v>0.2561913765432099</v>
       </c>
       <c r="H9">
-        <v>3.320210405974267</v>
+        <v>3.186615658675711</v>
       </c>
       <c r="I9">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J9">
-        <v>0.5432936760891717</v>
+        <v>0.7554661938984805</v>
       </c>
       <c r="K9">
-        <v>0.3175620943637407</v>
+        <v>0.3350485440787231</v>
       </c>
       <c r="L9">
-        <v>0.08626473881672655</v>
+        <v>0.1265589241831901</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -805,31 +805,31 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>2.171</v>
+        <v>1.031</v>
       </c>
       <c r="E10">
-        <v>2.5</v>
+        <v>2.95</v>
       </c>
       <c r="F10">
-        <v>1.511555555555556</v>
+        <v>1.694111111111111</v>
       </c>
       <c r="G10">
-        <v>0.2361455246913581</v>
+        <v>0.2561913765432099</v>
       </c>
       <c r="H10">
-        <v>3.660912673014101</v>
+        <v>3.848807092651113</v>
       </c>
       <c r="I10">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J10">
-        <v>0.3269181042678244</v>
+        <v>0.3341374974572674</v>
       </c>
       <c r="K10">
-        <v>0.2080379773195763</v>
+        <v>0.255206917186555</v>
       </c>
       <c r="L10">
-        <v>0.03400569058051426</v>
+        <v>0.04263710032124978</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -843,31 +843,31 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1.027</v>
+        <v>1.742</v>
       </c>
       <c r="E11">
-        <v>1.7</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>1.511555555555556</v>
+        <v>1.694111111111111</v>
       </c>
       <c r="G11">
-        <v>0.2361455246913581</v>
+        <v>0.2561913765432099</v>
       </c>
       <c r="H11">
-        <v>3.306904141230659</v>
+        <v>3.267908746498724</v>
       </c>
       <c r="I11">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J11">
-        <v>0.4993622153895869</v>
+        <v>0.7846644510953596</v>
       </c>
       <c r="K11">
-        <v>0.1367867395911887</v>
+        <v>0.3363547285902926</v>
       </c>
       <c r="L11">
-        <v>0.03415306465908726</v>
+        <v>0.1319627992413153</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -881,31 +881,31 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>1.2415</v>
+        <v>2.302</v>
       </c>
       <c r="E12">
-        <v>2.95</v>
+        <v>1.7</v>
       </c>
       <c r="F12">
-        <v>1.511555555555556</v>
+        <v>1.694111111111111</v>
       </c>
       <c r="G12">
-        <v>0.2361455246913581</v>
+        <v>0.2561913765432099</v>
       </c>
       <c r="H12">
-        <v>3.373280740940054</v>
+        <v>2.810379810007391</v>
       </c>
       <c r="I12">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J12">
-        <v>0.7034893675665789</v>
+        <v>0.3831915621817934</v>
       </c>
       <c r="K12">
-        <v>0.3094027247731894</v>
+        <v>0.2175938845554888</v>
       </c>
       <c r="L12">
-        <v>0.1088307635870336</v>
+        <v>0.04169007027201128</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -919,31 +919,31 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1.166</v>
+        <v>1.2415</v>
       </c>
       <c r="E13">
-        <v>1.8</v>
+        <v>4.9</v>
       </c>
       <c r="F13">
-        <v>1.511555555555556</v>
+        <v>1.694111111111111</v>
       </c>
       <c r="G13">
-        <v>0.2361455246913581</v>
+        <v>0.2561913765432099</v>
       </c>
       <c r="H13">
-        <v>3.349917415634416</v>
+        <v>3.676825233487854</v>
       </c>
       <c r="I13">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J13">
-        <v>0.63755576865018</v>
+        <v>0.5284350661159578</v>
       </c>
       <c r="K13">
-        <v>0.1454058552680375</v>
+        <v>0.1971378608669609</v>
       </c>
       <c r="L13">
-        <v>0.04635217091082524</v>
+        <v>0.05208727927059548</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -957,31 +957,31 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>1.8415</v>
+        <v>1.07</v>
       </c>
       <c r="E14">
-        <v>2.9</v>
+        <v>4.25</v>
       </c>
       <c r="F14">
-        <v>1.511555555555556</v>
+        <v>1.694111111111111</v>
       </c>
       <c r="G14">
-        <v>0.2361455246913581</v>
+        <v>0.2561913765432099</v>
       </c>
       <c r="H14">
-        <v>3.558949551315985</v>
+        <v>3.816943470288324</v>
       </c>
       <c r="I14">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J14">
-        <v>0.6519512142755522</v>
+        <v>0.3685327064981622</v>
       </c>
       <c r="K14">
-        <v>0.2837266749816377</v>
+        <v>0.3220624641982008</v>
       </c>
       <c r="L14">
-        <v>0.09248797513832181</v>
+        <v>0.0593452757962152</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -995,31 +995,31 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>1.239</v>
+        <v>2.446</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>2.55</v>
       </c>
       <c r="F15">
-        <v>1.511555555555556</v>
+        <v>1.694111111111111</v>
       </c>
       <c r="G15">
-        <v>0.2361455246913581</v>
+        <v>0.2561913765432099</v>
       </c>
       <c r="H15">
-        <v>3.372507120896821</v>
+        <v>2.692729512052477</v>
       </c>
       <c r="I15">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J15">
-        <v>0.7014716844176307</v>
+        <v>0.2614866445343001</v>
       </c>
       <c r="K15">
-        <v>0.3136783699910016</v>
+        <v>0.3429027718760512</v>
       </c>
       <c r="L15">
-        <v>0.1100182472814824</v>
+        <v>0.0448322476096896</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1036,28 +1036,28 @@
         <v>1.402</v>
       </c>
       <c r="E16">
-        <v>2.55</v>
+        <v>5.5</v>
       </c>
       <c r="F16">
-        <v>1.511555555555556</v>
+        <v>1.694111111111111</v>
       </c>
       <c r="G16">
-        <v>0.2361455246913581</v>
+        <v>0.2561913765432099</v>
       </c>
       <c r="H16">
-        <v>3.422947147715615</v>
+        <v>3.545694172225605</v>
       </c>
       <c r="I16">
-        <v>1.472012656008563</v>
+        <v>1.333033786264961</v>
       </c>
       <c r="J16">
-        <v>0.8003563595122321</v>
+        <v>0.6672724976589723</v>
       </c>
       <c r="K16">
-        <v>0.2538287093072221</v>
+        <v>0.08247741402644236</v>
       </c>
       <c r="L16">
-        <v>0.1015767108604085</v>
+        <v>0.02751745502893868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>